<commit_message>
2 June 2023 Selenium Grid
</commit_message>
<xml_diff>
--- a/src/test/resources/Materials/TestCasesTemplate.xlsx
+++ b/src/test/resources/Materials/TestCasesTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\softstandard oct 2021 batch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\SSMarchSeleniumJava2023\src\test\resources\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A56D4D7-78AC-470A-82CB-F16E1EAEC676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A1D232-C129-4548-849C-045AF11EAA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{F7EE1F96-14DD-413D-B06F-D2A58A0C4D07}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F7EE1F96-14DD-413D-B06F-D2A58A0C4D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>Application</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>User should be able to view replacement policy in days under product delivery etsimation in cart page</t>
-  </si>
-  <si>
-    <t>Block</t>
   </si>
   <si>
     <t>Priority</t>
@@ -304,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -314,62 +311,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,47 +678,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACFE7F4-EF15-441E-803F-E4F3B0A9ECA8}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.9296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.06640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.19921875" customWidth="1"/>
-    <col min="12" max="12" width="11.06640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.1796875" customWidth="1"/>
+    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
@@ -757,648 +748,612 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="21">
+        <v>44621</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="12">
-        <v>44621</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="11">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="14">
-        <v>78523</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="16" t="s">
+      <c r="N2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="10"/>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="17"/>
-    </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="10"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="17"/>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="17"/>
-    </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="10"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="17"/>
-    </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="6" t="s">
-        <v>53</v>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="19"/>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="12"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="21">
         <v>44621</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="11">
+      <c r="G8" s="13">
         <v>2</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="14" t="s">
         <v>27</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="O8" s="14" t="s">
+      <c r="N8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="P8" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="10"/>
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="17"/>
-    </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="10"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="11"/>
+    </row>
+    <row r="10" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="17"/>
-    </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="10"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="17"/>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="10"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="17"/>
-    </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="10"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="11"/>
+    </row>
+    <row r="13" spans="1:16" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="17"/>
-    </row>
-    <row r="14" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="17">
         <v>44621</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="11" t="s">
+      <c r="E14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="13">
+        <v>3</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="11">
-        <v>3</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>49</v>
+      <c r="J14" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="M14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="7">
         <v>78529</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P14" s="16" t="s">
+      <c r="P14" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="5" t="s">
+    <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="17"/>
-    </row>
-    <row r="16" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="5" t="s">
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="11"/>
+    </row>
+    <row r="16" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="17"/>
-    </row>
-    <row r="17" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="5" t="s">
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="11"/>
+    </row>
+    <row r="17" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="17"/>
-    </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="10"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="11"/>
+    </row>
+    <row r="18" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="11"/>
+    </row>
+    <row r="19" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="17">
+        <v>44621</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="13">
+        <v>4</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="17"/>
-    </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="20">
-        <v>44621</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="11">
-        <v>4</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="N19" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="O19" s="14" t="s">
+      <c r="O19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P19" s="16" t="s">
+      <c r="P19" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="5" t="s">
+    <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="17"/>
-    </row>
-    <row r="21" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="5" t="s">
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="11"/>
+    </row>
+    <row r="21" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="17"/>
-    </row>
-    <row r="22" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="5" t="s">
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="11"/>
+    </row>
+    <row r="22" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="17"/>
-    </row>
-    <row r="23" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="10"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="11"/>
+    </row>
+    <row r="23" spans="1:16" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="11"/>
+    </row>
+    <row r="24" spans="1:16" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="17"/>
-    </row>
-    <row r="24" spans="1:16" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="17"/>
-    </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="5"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="11"/>
+    </row>
+    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="3"/>
       <c r="K25" s="4"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="19"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="N19:N25"/>
-    <mergeCell ref="O19:O25"/>
-    <mergeCell ref="P19:P25"/>
-    <mergeCell ref="F19:F25"/>
-    <mergeCell ref="G19:G25"/>
-    <mergeCell ref="H19:H25"/>
-    <mergeCell ref="I19:I25"/>
-    <mergeCell ref="M19:M25"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="C19:C25"/>
-    <mergeCell ref="D19:D25"/>
-    <mergeCell ref="E19:E25"/>
-    <mergeCell ref="E2:E7"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="M14:M18"/>
-    <mergeCell ref="N14:N18"/>
-    <mergeCell ref="O14:O18"/>
-    <mergeCell ref="P14:P18"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="D14:D18"/>
-    <mergeCell ref="H14:H18"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="N8:N13"/>
-    <mergeCell ref="O8:O13"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="M2:M7"/>
-    <mergeCell ref="N2:N7"/>
-    <mergeCell ref="O2:O7"/>
-    <mergeCell ref="P2:P7"/>
     <mergeCell ref="I8:I13"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
@@ -1415,6 +1370,42 @@
     <mergeCell ref="G2:G7"/>
     <mergeCell ref="F8:F13"/>
     <mergeCell ref="G8:G13"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="N8:N13"/>
+    <mergeCell ref="O8:O13"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="M2:M7"/>
+    <mergeCell ref="N2:N7"/>
+    <mergeCell ref="O2:O7"/>
+    <mergeCell ref="P2:P7"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="M14:M18"/>
+    <mergeCell ref="N14:N18"/>
+    <mergeCell ref="O14:O18"/>
+    <mergeCell ref="P14:P18"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="C19:C25"/>
+    <mergeCell ref="D19:D25"/>
+    <mergeCell ref="E19:E25"/>
+    <mergeCell ref="N19:N25"/>
+    <mergeCell ref="O19:O25"/>
+    <mergeCell ref="P19:P25"/>
+    <mergeCell ref="F19:F25"/>
+    <mergeCell ref="G19:G25"/>
+    <mergeCell ref="H19:H25"/>
+    <mergeCell ref="I19:I25"/>
+    <mergeCell ref="M19:M25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1427,7 +1418,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1439,7 +1430,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>